<commit_message>
Refactor - SRLV species level, genome-length alignment and corresponding phylogeny build
</commit_message>
<xml_diff>
--- a/tabular/core/lenti-reference-data.xlsx
+++ b/tabular/core/lenti-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Lentivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A665782-7D9A-774C-8A13-EB23D329CA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBEC40E-FDF3-D747-925B-75E83AB76A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8120" yWindow="9980" windowWidth="24900" windowHeight="11960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="590">
   <si>
     <t>Accession</t>
   </si>
@@ -1797,6 +1797,9 @@
   </si>
   <si>
     <t>HIV-1M</t>
+  </si>
+  <si>
+    <t>Iceland</t>
   </si>
 </sst>
 </file>
@@ -2378,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B72CCB-88DE-2049-8047-9EF1763B24DD}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="A1:M6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2595,6 +2598,9 @@
       </c>
       <c r="J6" t="s">
         <v>450</v>
+      </c>
+      <c r="M6" t="s">
+        <v>589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added genome feature details
</commit_message>
<xml_diff>
--- a/tabular/core/lenti-reference-data.xlsx
+++ b/tabular/core/lenti-reference-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Lentivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199E0DE4-7F72-504E-9FF9-5BA20FEE7ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664BF2E2-46B2-5E40-A8A8-20C7851D2826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25400" yWindow="6360" windowWidth="24900" windowHeight="11960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="1260" windowWidth="36480" windowHeight="23560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="612">
   <si>
     <t>Accession</t>
   </si>
@@ -1809,13 +1809,70 @@
   </si>
   <si>
     <t>NK</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIVpco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIVoma </t>
+  </si>
+  <si>
+    <t>KU168292</t>
+  </si>
+  <si>
+    <t>LA49RBF189</t>
+  </si>
+  <si>
+    <t>GU111555</t>
+  </si>
+  <si>
+    <t>RBF168</t>
+  </si>
+  <si>
+    <t>JN835461</t>
+  </si>
+  <si>
+    <t>Chimpanzee</t>
+  </si>
+  <si>
+    <t>JN835460</t>
+  </si>
+  <si>
+    <t>SIVcpzEK505.c2</t>
+  </si>
+  <si>
+    <t>EF394356</t>
+  </si>
+  <si>
+    <t>pts</t>
+  </si>
+  <si>
+    <t>SIVcpzTAN1</t>
+  </si>
+  <si>
+    <t>SIVgor-BQID2</t>
+  </si>
+  <si>
+    <t>SIVgor-BPID15</t>
+  </si>
+  <si>
+    <t>pubmed_id</t>
+  </si>
+  <si>
+    <t>Simian immunodeficiency virus cpz</t>
+  </si>
+  <si>
+    <t>Simian immunodeficiency virus gor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1884,8 +1941,22 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1940,6 +2011,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1977,7 +2054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2036,15 +2113,34 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2394,270 +2490,678 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B72CCB-88DE-2049-8047-9EF1763B24DD}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M6" sqref="A1:M6"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="14"/>
     <col min="9" max="9" width="25.1640625" customWidth="1"/>
     <col min="10" max="10" width="23.1640625" customWidth="1"/>
     <col min="12" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>456</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>455</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>585</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="31" t="s">
         <v>461</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>579</v>
       </c>
       <c r="H1" s="31" t="s">
         <v>586</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="31" t="s">
         <v>570</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="31" t="s">
         <v>571</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="31" t="s">
         <v>572</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="31" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="N1" s="31" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>581</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>500</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>501</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>501</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>581</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>502</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>503</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M3" s="34" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>578</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="G4" s="30">
+        <v>1</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>528</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>582</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M7" s="28"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>587</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="M8" s="28"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B9" s="28" t="s">
         <v>576</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C9" s="28" t="s">
         <v>588</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D9" s="28" t="s">
         <v>580</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E9" s="28" t="s">
         <v>473</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F9" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H9" s="28" t="s">
         <v>587</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I9" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J9" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L9" s="28" t="s">
         <v>592</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M9" s="28" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" t="s">
-        <v>463</v>
-      </c>
-      <c r="C3" t="s">
-        <v>325</v>
-      </c>
-      <c r="D3" t="s">
-        <v>325</v>
-      </c>
-      <c r="E3" t="s">
-        <v>581</v>
-      </c>
-      <c r="F3" t="s">
-        <v>574</v>
-      </c>
-      <c r="G3" t="s">
-        <v>574</v>
-      </c>
-      <c r="H3" s="14" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="D10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="I10" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>438</v>
+      </c>
+      <c r="L10" s="38">
+        <v>1995</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="38">
+        <v>9734396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>596</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>597</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="I11" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>438</v>
+      </c>
+      <c r="L11" s="38">
+        <v>2005</v>
+      </c>
+      <c r="M11" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="38">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>598</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>599</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="I12" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>438</v>
+      </c>
+      <c r="L12" s="38">
+        <v>2009</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="38" t="s">
         <v>587</v>
       </c>
-      <c r="I3" t="s">
-        <v>469</v>
-      </c>
-      <c r="J3" t="s">
-        <v>436</v>
-      </c>
-      <c r="K3" t="s">
-        <v>592</v>
-      </c>
-      <c r="L3" t="s">
-        <v>592</v>
-      </c>
-      <c r="M3" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>336</v>
-      </c>
-      <c r="B4" t="s">
-        <v>569</v>
-      </c>
-      <c r="C4" t="s">
-        <v>337</v>
-      </c>
-      <c r="D4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E4" t="s">
-        <v>582</v>
-      </c>
-      <c r="F4" t="s">
-        <v>575</v>
-      </c>
-      <c r="G4" t="s">
-        <v>575</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>587</v>
-      </c>
-      <c r="I4" t="s">
-        <v>479</v>
-      </c>
-      <c r="J4" t="s">
-        <v>480</v>
-      </c>
-      <c r="K4" t="s">
-        <v>592</v>
-      </c>
-      <c r="L4" t="s">
-        <v>592</v>
-      </c>
-      <c r="M4" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>328</v>
-      </c>
-      <c r="B5" t="s">
-        <v>482</v>
-      </c>
-      <c r="C5" t="s">
-        <v>383</v>
-      </c>
-      <c r="D5" t="s">
-        <v>383</v>
-      </c>
-      <c r="E5" t="s">
-        <v>583</v>
-      </c>
-      <c r="F5" t="s">
-        <v>574</v>
-      </c>
-      <c r="G5" t="s">
-        <v>574</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>587</v>
-      </c>
-      <c r="I5" t="s">
-        <v>493</v>
-      </c>
-      <c r="J5" t="s">
-        <v>434</v>
-      </c>
-      <c r="K5" t="s">
-        <v>592</v>
-      </c>
-      <c r="L5" t="s">
-        <v>592</v>
-      </c>
-      <c r="M5" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>578</v>
-      </c>
-      <c r="B6" t="s">
-        <v>577</v>
-      </c>
-      <c r="C6" t="s">
-        <v>343</v>
-      </c>
-      <c r="D6" t="s">
-        <v>388</v>
-      </c>
-      <c r="E6" t="s">
-        <v>584</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="33">
-        <v>1</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="I6" t="s">
-        <v>528</v>
-      </c>
-      <c r="J6" t="s">
-        <v>450</v>
-      </c>
-      <c r="K6" t="s">
-        <v>592</v>
-      </c>
-      <c r="L6" t="s">
-        <v>592</v>
-      </c>
-      <c r="M6" t="s">
-        <v>589</v>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>600</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>610</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="I13" s="38" t="s">
+        <v>601</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N13" s="38">
+        <v>22505456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>602</v>
+      </c>
+      <c r="B14" t="s">
+        <v>610</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>603</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="I14" s="38" t="s">
+        <v>601</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N14" s="38">
+        <v>22505456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>604</v>
+      </c>
+      <c r="B15" t="s">
+        <v>610</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>606</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>605</v>
+      </c>
+      <c r="G15" s="38"/>
+      <c r="I15" s="38" t="s">
+        <v>601</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="38">
+        <v>17494082</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s">
+        <v>611</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>550</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>607</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="G16" s="38"/>
+      <c r="I16" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="L16" s="38">
+        <v>2012</v>
+      </c>
+      <c r="M16" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" s="38">
+        <v>25733890</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" t="s">
+        <v>611</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>550</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>608</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="G17" s="38"/>
+      <c r="I17" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="L17" s="38">
+        <v>2013</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="38">
+        <v>25733890</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M9">
+    <sortCondition ref="E2:E9"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Detailed feature annotations added to paleoviruses
</commit_message>
<xml_diff>
--- a/tabular/core/lenti-reference-data.xlsx
+++ b/tabular/core/lenti-reference-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Lentivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9C9C57-9E02-144B-B10F-CB933C6A9291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FCBF9B-2E3E-C343-9D7C-0E72194031F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="2880" windowWidth="36480" windowHeight="23560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12780" yWindow="3500" windowWidth="36480" windowHeight="23560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="659">
   <si>
     <t>Accession</t>
   </si>
@@ -1895,18 +1895,9 @@
     <t>AF322109</t>
   </si>
   <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
     <t>JF502416</t>
   </si>
   <si>
-    <t>B3</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -2010,6 +2001,12 @@
   </si>
   <si>
     <t>Collared mangabey</t>
+  </si>
+  <si>
+    <t>Seui</t>
+  </si>
+  <si>
+    <t>Feline immunodeficiency virus isolate SR631</t>
   </si>
 </sst>
 </file>
@@ -2641,7 +2638,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:N36"/>
+      <selection activeCell="B15" sqref="A1:N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2812,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>448</v>
+        <v>587</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>528</v>
@@ -2856,7 +2853,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>8</v>
+        <v>587</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>614</v>
@@ -2879,13 +2876,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>388</v>
@@ -2894,13 +2891,13 @@
         <v>584</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G6" s="30">
         <v>2</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>621</v>
+        <v>657</v>
       </c>
       <c r="I6" s="28" t="s">
         <v>614</v>
@@ -2915,7 +2912,7 @@
         <v>592</v>
       </c>
       <c r="M6" s="28" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>592</v>
@@ -2926,10 +2923,10 @@
         <v>619</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>388</v>
@@ -2938,13 +2935,13 @@
         <v>584</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G7" s="30">
         <v>1</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>622</v>
+        <v>587</v>
       </c>
       <c r="I7" s="28" t="s">
         <v>614</v>
@@ -2959,7 +2956,7 @@
         <v>592</v>
       </c>
       <c r="M7" s="28" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="N7" s="28" t="s">
         <v>592</v>
@@ -2970,10 +2967,10 @@
         <v>620</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>388</v>
@@ -2988,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>47</v>
+        <v>587</v>
       </c>
       <c r="I8" s="28" t="s">
         <v>614</v>
@@ -3003,7 +3000,7 @@
         <v>592</v>
       </c>
       <c r="M8" s="28" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="N8" s="28" t="s">
         <v>592</v>
@@ -3011,13 +3008,13 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>388</v>
@@ -3032,7 +3029,7 @@
         <v>3</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>624</v>
+        <v>587</v>
       </c>
       <c r="I9" s="28" t="s">
         <v>614</v>
@@ -3047,7 +3044,7 @@
         <v>592</v>
       </c>
       <c r="M9" s="28" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="N9" s="28" t="s">
         <v>592</v>
@@ -3075,8 +3072,8 @@
       <c r="G10" s="36" t="s">
         <v>575</v>
       </c>
-      <c r="H10" s="36" t="s">
-        <v>575</v>
+      <c r="H10" s="41" t="s">
+        <v>587</v>
       </c>
       <c r="I10" s="36" t="s">
         <v>479</v>
@@ -3119,8 +3116,8 @@
       <c r="G11" s="36" t="s">
         <v>617</v>
       </c>
-      <c r="H11" s="36" t="s">
-        <v>617</v>
+      <c r="H11" s="41" t="s">
+        <v>587</v>
       </c>
       <c r="I11" s="36" t="s">
         <v>479</v>
@@ -3162,7 +3159,7 @@
         <v>616</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>616</v>
+        <v>587</v>
       </c>
       <c r="I12" s="36" t="s">
         <v>479</v>
@@ -3230,7 +3227,7 @@
         <v>481</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>482</v>
+        <v>658</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>594</v>
@@ -3262,7 +3259,9 @@
       <c r="L14" s="28" t="s">
         <v>592</v>
       </c>
-      <c r="M14" s="28"/>
+      <c r="M14" s="28" t="s">
+        <v>592</v>
+      </c>
       <c r="N14" s="28" t="s">
         <v>592</v>
       </c>
@@ -3304,7 +3303,9 @@
       <c r="L15" s="28" t="s">
         <v>592</v>
       </c>
-      <c r="M15" s="28"/>
+      <c r="M15" s="28" t="s">
+        <v>592</v>
+      </c>
       <c r="N15" s="28" t="s">
         <v>592</v>
       </c>
@@ -3635,7 +3636,7 @@
         <v>587</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="J23" s="40" t="s">
         <v>398</v>
@@ -3679,7 +3680,7 @@
         <v>587</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="J24" s="40" t="s">
         <v>398</v>
@@ -3702,7 +3703,7 @@
         <v>208</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C25" s="40" t="s">
         <v>538</v>
@@ -3723,7 +3724,7 @@
         <v>587</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="J25" s="40" t="s">
         <v>408</v>
@@ -3740,7 +3741,7 @@
         <v>197</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C26" s="40" t="s">
         <v>537</v>
@@ -3779,10 +3780,10 @@
         <v>504</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E27" s="36" t="s">
         <v>473</v>
@@ -3812,7 +3813,7 @@
         <v>357</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C28" s="40" t="s">
         <v>358</v>
@@ -3833,10 +3834,10 @@
         <v>587</v>
       </c>
       <c r="I28" s="40" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="J28" s="41" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="K28" s="40"/>
       <c r="L28" s="40"/>
@@ -3848,7 +3849,7 @@
         <v>170</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>540</v>
@@ -3869,7 +3870,7 @@
         <v>587</v>
       </c>
       <c r="I29" s="41" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="J29" s="41" t="s">
         <v>400</v>
@@ -3884,7 +3885,7 @@
         <v>346</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>347</v>
@@ -3905,7 +3906,7 @@
         <v>587</v>
       </c>
       <c r="I30" s="41" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="J30" s="41" t="s">
         <v>410</v>
@@ -3917,7 +3918,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B31" s="37" t="s">
         <v>564</v>
@@ -3956,7 +3957,7 @@
         <v>218</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>534</v>
@@ -3977,7 +3978,7 @@
         <v>587</v>
       </c>
       <c r="I32" s="40" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="J32" s="41" t="s">
         <v>411</v>
@@ -3992,13 +3993,13 @@
         <v>143</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E33" s="36" t="s">
         <v>473</v>
@@ -4013,7 +4014,7 @@
         <v>587</v>
       </c>
       <c r="I33" s="41" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="J33" s="41" t="s">
         <v>396</v>
@@ -4028,13 +4029,13 @@
         <v>210</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E34" s="36" t="s">
         <v>473</v>
@@ -4064,7 +4065,7 @@
         <v>349</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C35" s="40" t="s">
         <v>350</v>
@@ -4085,7 +4086,7 @@
         <v>587</v>
       </c>
       <c r="I35" s="41" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="J35" s="40" t="s">
         <v>547</v>
@@ -4103,10 +4104,10 @@
         <v>504</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E36" s="36" t="s">
         <v>473</v>

</xml_diff>

<commit_message>
Added HIV-2 reference (incomplete annotation)
</commit_message>
<xml_diff>
--- a/tabular/core/lenti-reference-data.xlsx
+++ b/tabular/core/lenti-reference-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Lentivirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E6774-6733-4A4A-8FAA-C0C457F8A302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E50B4A-41AF-734C-A0E1-33EBCF8EB93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="1940" windowWidth="36480" windowHeight="23560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="2820" windowWidth="36480" windowHeight="23560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="653">
   <si>
     <t>Accession</t>
   </si>
@@ -1985,6 +1985,9 @@
   </si>
   <si>
     <t>Ovine-Caprine</t>
+  </si>
+  <si>
+    <t>X05291</t>
   </si>
 </sst>
 </file>
@@ -2600,10 +2603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B72CCB-88DE-2049-8047-9EF1763B24DD}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="B26" sqref="A1:N37"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4240,6 +4243,50 @@
         <v>582</v>
       </c>
       <c r="N37" s="37" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="35" t="s">
+        <v>652</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>555</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>464</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>577</v>
+      </c>
+      <c r="H38" s="38" t="s">
+        <v>577</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>488</v>
+      </c>
+      <c r="J38" s="38" t="s">
+        <v>312</v>
+      </c>
+      <c r="K38" s="37" t="s">
+        <v>582</v>
+      </c>
+      <c r="L38" s="37" t="s">
+        <v>582</v>
+      </c>
+      <c r="M38" s="37" t="s">
+        <v>582</v>
+      </c>
+      <c r="N38" s="37" t="s">
         <v>582</v>
       </c>
     </row>

</xml_diff>